<commit_message>
Atualizando via Git GUI no W-10: 2023/03/22.
</commit_message>
<xml_diff>
--- a/dados/COVID19IES.xlsx
+++ b/dados/COVID19IES.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\with-a-little-help-from-my-friends\dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jpalbino/Library/Mobile Documents/com~apple~CloudDocs/GitHub/with-a-little-help-from-my-friends/dados/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED27940-5362-4F60-817F-14E15426EB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E245214E-00C7-064B-BB9F-B4776ABF1D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2352" yWindow="1452" windowWidth="18972" windowHeight="11016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Respostas ao formulário 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2252" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2262" uniqueCount="394">
   <si>
     <t>Sim</t>
   </si>
@@ -609,9 +609,6 @@
     <t>Meu ingresso foi em 2022, portanto não tenho vivência academia durante a pandemia.</t>
   </si>
   <si>
-    <t>Não se aplica / Não sabe</t>
-  </si>
-  <si>
     <t>Aposentei-me em 01.02.2020, passei pelo confinamento junto com meu marido. Foram dias difíceis, de pouca ou quase nenhuma convivência social. Mesmo com a 3a. dose da vacina, ainda tenho insegurança sem as máscaras e a volta ao "normal". Infelizmente, em 19.11.2021, meu esposo foi vítima de um atropelador irresponsável e veio a falecer. Desde então conto com acompanhamento psicológico profissional. Em 2022 ingressei como mestranda no Curso de Pós-Graduação. Sinto falta da convivência acadêmica, mas tenho preocupação em me expor ao vírus e as consequências da doença.</t>
   </si>
   <si>
@@ -897,15 +894,6 @@
     <t xml:space="preserve">Bacharelado em Sistemas de Informação </t>
   </si>
   <si>
-    <t>É mais ou menos o mesmo</t>
-  </si>
-  <si>
-    <t>São mais ou menos os mesmos</t>
-  </si>
-  <si>
-    <t>São mais ou menos as mesmas</t>
-  </si>
-  <si>
     <t>Reconheço que minha instituição foi muito receptiva a dificuldade e dúvidas que os alunos tiveram ao longo do processo.</t>
   </si>
   <si>
@@ -918,9 +906,6 @@
     <t>Fundação Getúlio Vargas</t>
   </si>
   <si>
-    <t>Está mais ou menos o mesmo</t>
-  </si>
-  <si>
     <t>Não presenciei a alteração de dinâmica durante o curso (ingressei em 2021 na instituição), porém acredito que a produtividade aumentou. Atualmente tenho mais tempo focado na realização das tarefas que anteriormente.</t>
   </si>
   <si>
@@ -939,9 +924,6 @@
     <t>Reconhecendo o privilégio de poder trabalhar e estudar da minha casa, acredito que a pandemia impactou pouco meu cotidiano em questões econômicas ou de saúde. Uma observação possível é que a utilização do tempo melhorou. Mais atividades podem ser realizadas ao mesmo momento. Por outro lado, aspectos como distanciamento social e  incertezas sobre os meses futuros impactaram diretamente o psicológico.</t>
   </si>
   <si>
-    <t>Está/É mais ou menos o mesmo</t>
-  </si>
-  <si>
     <t>Alimentação, Outras (por favor, complemente):</t>
   </si>
   <si>
@@ -957,9 +939,6 @@
     <t>trabalhasse com prazos mais flexíveis de entregas e conclusões.</t>
   </si>
   <si>
-    <t>Sim, completamente vacinado com duas doses ou com vacina de dose única</t>
-  </si>
-  <si>
     <t>Alguns professores, que prefiro não mencionar, não se encontram disponíveis para consulta. Isto é, não permitiram/permitem perguntas durante suas aulas síncronas e não estão disponíveis para consulta fora delas. Ou seja, não é possível sanar dúvidas de suas matérias diretamente sendo necessário buscar respostas independentemente. Entendo que a capacidade de estudar independentemente seja importante mas isso não significa que os professores possam simplesmente ignorar as dúvidas dos alunos sobre as matérias que lecionam. Fora isso, alguns colegas possuem dificuldades decorrentes de má disponibilidade de internet. Sendo incapazes, por exemplo, de manterem-se conectados por 4 horas consecutivas às aulas síncronas.</t>
   </si>
   <si>
@@ -1026,9 +1005,6 @@
     <t>moradia_atual_permanente</t>
   </si>
   <si>
-    <t>morando_ com</t>
-  </si>
-  <si>
     <t xml:space="preserve"> convive_risco_relevante</t>
   </si>
   <si>
@@ -1047,12 +1023,6 @@
     <t>capacidade_prosseguir_estudos</t>
   </si>
   <si>
-    <t xml:space="preserve">capacidade_ socializacao </t>
-  </si>
-  <si>
-    <t>bem-estar_psicologico</t>
-  </si>
-  <si>
     <t>aulas_durante_pandemia</t>
   </si>
   <si>
@@ -1098,9 +1068,6 @@
     <t>nivel_endividamento</t>
   </si>
   <si>
-    <t>despesas_ cresceram</t>
-  </si>
-  <si>
     <t>dificuldades_financeiras</t>
   </si>
   <si>
@@ -1110,9 +1077,6 @@
     <t>ies_positivo</t>
   </si>
   <si>
-    <t>ies_ melhorar</t>
-  </si>
-  <si>
     <t>ies_ajudar</t>
   </si>
   <si>
@@ -1222,13 +1186,31 @@
   </si>
   <si>
     <t>nivel_ensino</t>
+  </si>
+  <si>
+    <t>morando_com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capacidade_socializacao </t>
+  </si>
+  <si>
+    <t>bem_estar_psicologico</t>
+  </si>
+  <si>
+    <t>despesas_cresceram</t>
+  </si>
+  <si>
+    <t>ies_melhorar</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1507,220 +1489,223 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BB53"/>
+  <dimension ref="A1:BB54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AZ54" sqref="AZ54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="10.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.5" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="40.109375" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="40.1640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="7" max="7" width="33.33203125" customWidth="1"/>
-    <col min="8" max="8" width="57.21875" customWidth="1"/>
+    <col min="8" max="8" width="57.1640625" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="15.1640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="7.33203125" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" customWidth="1"/>
-    <col min="14" max="14" width="14.44140625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="11.5" customWidth="1"/>
+    <col min="14" max="14" width="14.5" customWidth="1"/>
     <col min="15" max="15" width="100.33203125" customWidth="1"/>
     <col min="16" max="16" width="14" style="3" customWidth="1"/>
-    <col min="17" max="17" width="60.88671875" customWidth="1"/>
-    <col min="18" max="20" width="18.88671875" customWidth="1"/>
-    <col min="21" max="21" width="16.77734375" customWidth="1"/>
-    <col min="22" max="22" width="102.109375" customWidth="1"/>
-    <col min="23" max="26" width="18.88671875" customWidth="1"/>
-    <col min="27" max="27" width="22.88671875" customWidth="1"/>
-    <col min="28" max="28" width="18.88671875" customWidth="1"/>
-    <col min="29" max="29" width="28.88671875" customWidth="1"/>
-    <col min="30" max="30" width="28.44140625" customWidth="1"/>
+    <col min="17" max="17" width="60.83203125" customWidth="1"/>
+    <col min="18" max="20" width="18.83203125" customWidth="1"/>
+    <col min="21" max="21" width="16.83203125" customWidth="1"/>
+    <col min="22" max="22" width="102.1640625" customWidth="1"/>
+    <col min="23" max="23" width="32.1640625" customWidth="1"/>
+    <col min="24" max="24" width="18.83203125" customWidth="1"/>
+    <col min="25" max="25" width="27.1640625" customWidth="1"/>
+    <col min="26" max="27" width="22.83203125" customWidth="1"/>
+    <col min="28" max="28" width="18.83203125" customWidth="1"/>
+    <col min="29" max="29" width="28.83203125" customWidth="1"/>
+    <col min="30" max="30" width="28.5" customWidth="1"/>
     <col min="31" max="31" width="26.6640625" customWidth="1"/>
-    <col min="32" max="32" width="25.88671875" customWidth="1"/>
+    <col min="32" max="32" width="25.83203125" customWidth="1"/>
     <col min="33" max="33" width="27.6640625" customWidth="1"/>
     <col min="34" max="34" width="25.33203125" customWidth="1"/>
-    <col min="35" max="35" width="52.21875" customWidth="1"/>
-    <col min="36" max="36" width="10.44140625" customWidth="1"/>
+    <col min="35" max="35" width="52.1640625" customWidth="1"/>
+    <col min="36" max="36" width="11" customWidth="1"/>
     <col min="37" max="37" width="66.6640625" customWidth="1"/>
-    <col min="38" max="38" width="28.5546875" customWidth="1"/>
-    <col min="39" max="39" width="30.77734375" customWidth="1"/>
-    <col min="40" max="40" width="25.88671875" customWidth="1"/>
+    <col min="38" max="38" width="28.5" customWidth="1"/>
+    <col min="39" max="39" width="30.83203125" customWidth="1"/>
+    <col min="40" max="40" width="25.83203125" customWidth="1"/>
     <col min="41" max="41" width="14" customWidth="1"/>
-    <col min="42" max="42" width="29.109375" customWidth="1"/>
-    <col min="43" max="43" width="84.44140625" customWidth="1"/>
-    <col min="44" max="44" width="23.109375" customWidth="1"/>
+    <col min="42" max="42" width="29.1640625" customWidth="1"/>
+    <col min="43" max="43" width="84.5" customWidth="1"/>
+    <col min="44" max="44" width="23.1640625" customWidth="1"/>
     <col min="45" max="45" width="26.6640625" customWidth="1"/>
-    <col min="46" max="49" width="18.88671875" customWidth="1"/>
-    <col min="50" max="50" width="21.44140625" customWidth="1"/>
-    <col min="51" max="51" width="21.21875" customWidth="1"/>
-    <col min="52" max="58" width="18.88671875" customWidth="1"/>
+    <col min="46" max="48" width="18.83203125" customWidth="1"/>
+    <col min="49" max="49" width="24.83203125" customWidth="1"/>
+    <col min="50" max="50" width="21.5" customWidth="1"/>
+    <col min="51" max="51" width="27.33203125" customWidth="1"/>
+    <col min="52" max="58" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:52" ht="13">
       <c r="A1" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>320</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>334</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>335</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>336</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="AV1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="AO1" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="AS1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="AT1" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="AU1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="AV1" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW1" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="AX1" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="AY1" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="AZ1" s="1" t="s">
-        <v>367</v>
-      </c>
     </row>
-    <row r="2" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:52" ht="15.75" customHeight="1">
       <c r="A2" s="2">
         <v>44308.772397754627</v>
       </c>
@@ -1740,7 +1725,7 @@
         <v>156</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>77</v>
@@ -1794,22 +1779,28 @@
         <v>12</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE2" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>291</v>
+        <v>20</v>
       </c>
       <c r="AH2" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="AI2" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="AM2" s="1" t="s">
-        <v>292</v>
+        <v>62</v>
       </c>
       <c r="AN2" s="1" t="s">
         <v>25</v>
@@ -1818,22 +1809,22 @@
         <v>10</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AS2" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="AW2" s="1" t="s">
         <v>37</v>
@@ -1845,7 +1836,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:52" ht="15.75" customHeight="1">
       <c r="A3" s="2">
         <v>44308.918698055553</v>
       </c>
@@ -1862,10 +1853,10 @@
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>33</v>
@@ -1892,7 +1883,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>10</v>
@@ -1919,10 +1910,13 @@
         <v>12</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="AF3" s="1" t="s">
         <v>80</v>
@@ -1931,10 +1925,13 @@
         <v>38</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI3" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="AM3" s="1" t="s">
         <v>24</v>
@@ -1952,19 +1949,19 @@
         <v>63</v>
       </c>
       <c r="AR3" s="1" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="AS3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT3" s="1" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="AU3" s="1" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="AV3" s="1" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="AW3" s="1" t="s">
         <v>15</v>
@@ -1976,10 +1973,10 @@
         <v>15</v>
       </c>
       <c r="AZ3" s="1" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:52" ht="15.75" customHeight="1">
       <c r="A4" s="2">
         <v>44312.609396006941</v>
       </c>
@@ -1999,7 +1996,7 @@
         <v>156</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
@@ -2056,19 +2053,25 @@
         <v>12</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD4" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE4" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF4" s="1" t="s">
         <v>80</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>291</v>
+        <v>20</v>
       </c>
       <c r="AH4" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI4" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AM4" s="1" t="s">
         <v>41</v>
@@ -2080,25 +2083,25 @@
         <v>10</v>
       </c>
       <c r="AP4" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ4" s="1" t="s">
-        <v>306</v>
+        <v>300</v>
       </c>
       <c r="AR4" s="1" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="AS4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT4" s="1" t="s">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="AU4" s="1" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="AV4" s="1" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="AW4" s="1" t="s">
         <v>12</v>
@@ -2110,7 +2113,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:52" ht="14">
       <c r="A5" s="2">
         <v>44337.639256956019</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>156</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>5</v>
@@ -2187,19 +2190,25 @@
         <v>37</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD5" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="AE5" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AF5" s="1" t="s">
-        <v>291</v>
+        <v>19</v>
       </c>
       <c r="AG5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="AH5" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="AM5" s="1" t="s">
         <v>24</v>
@@ -2211,7 +2220,7 @@
         <v>10</v>
       </c>
       <c r="AP5" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ5" s="1" t="s">
         <v>27</v>
@@ -2220,13 +2229,13 @@
         <v>28</v>
       </c>
       <c r="AT5" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="AU5" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="AV5" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="AW5" s="1" t="s">
         <v>37</v>
@@ -2238,7 +2247,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:52" ht="13">
       <c r="A6" s="2">
         <v>44490.349946111106</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>156</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>77</v>
@@ -2312,34 +2321,34 @@
         <v>37</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>305</v>
+        <v>16</v>
       </c>
       <c r="AD6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>291</v>
+        <v>19</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>291</v>
+        <v>20</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>298</v>
+        <v>21</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>311</v>
+        <v>40</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>292</v>
+        <v>62</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>42</v>
@@ -2348,16 +2357,16 @@
         <v>10</v>
       </c>
       <c r="AP6" s="1" t="s">
-        <v>293</v>
+        <v>26</v>
       </c>
       <c r="AQ6" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="AS6" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AU6" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="AW6" s="1" t="s">
         <v>15</v>
@@ -2369,7 +2378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:52" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:52" ht="13">
       <c r="A7" s="2">
         <v>44645.433733912039</v>
       </c>
@@ -2392,7 +2401,7 @@
         <v>156</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>5</v>
@@ -2497,7 +2506,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:52" ht="15.75" customHeight="1">
       <c r="A8" s="2">
         <v>44645.571748668983</v>
       </c>
@@ -2631,7 +2640,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:52" ht="15.75" customHeight="1">
       <c r="A9" s="2">
         <v>44645.603025405093</v>
       </c>
@@ -2774,7 +2783,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:52" ht="15.75" customHeight="1">
       <c r="A10" s="2">
         <v>44645.610024664347</v>
       </c>
@@ -2797,7 +2806,7 @@
         <v>156</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>33</v>
@@ -2929,7 +2938,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1">
       <c r="A11" s="2">
         <v>44645.984089571764</v>
       </c>
@@ -2952,7 +2961,7 @@
         <v>156</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>193</v>
@@ -2994,7 +3003,7 @@
         <v>10</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>37</v>
@@ -3012,10 +3021,10 @@
         <v>12</v>
       </c>
       <c r="AB11" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC11" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="AC11" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="AD11" s="1" t="s">
         <v>80</v>
@@ -3039,7 +3048,7 @@
         <v>174</v>
       </c>
       <c r="AL11" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="AM11" s="1" t="s">
         <v>41</v>
@@ -3054,22 +3063,22 @@
         <v>41</v>
       </c>
       <c r="AQ11" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="AR11" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="AR11" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="AS11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT11" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AU11" s="1" t="s">
         <v>194</v>
       </c>
       <c r="AV11" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AW11" s="1" t="s">
         <v>37</v>
@@ -3081,10 +3090,10 @@
         <v>37</v>
       </c>
       <c r="AZ11" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:52" ht="15.75" customHeight="1">
       <c r="A12" s="2">
         <v>44646.398636967591</v>
       </c>
@@ -3107,7 +3116,7 @@
         <v>156</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>5</v>
@@ -3128,7 +3137,7 @@
         <v>45</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P12" s="2">
         <v>43907</v>
@@ -3167,7 +3176,7 @@
         <v>12</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AC12" s="1" t="s">
         <v>16</v>
@@ -3197,7 +3206,7 @@
         <v>174</v>
       </c>
       <c r="AL12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="AM12" s="1" t="s">
         <v>41</v>
@@ -3212,22 +3221,22 @@
         <v>26</v>
       </c>
       <c r="AQ12" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="AR12" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="AR12" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="AS12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT12" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AU12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AV12" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AW12" s="1" t="s">
         <v>12</v>
@@ -3239,7 +3248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:52" ht="15.75" customHeight="1">
       <c r="A13" s="2">
         <v>44646.484321793978</v>
       </c>
@@ -3262,7 +3271,7 @@
         <v>156</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>33</v>
@@ -3361,13 +3370,13 @@
         <v>28</v>
       </c>
       <c r="AT13" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="AU13" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="AU13" s="1" t="s">
+      <c r="AV13" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="AV13" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="AW13" s="1" t="s">
         <v>15</v>
@@ -3379,7 +3388,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:52" ht="15.75" customHeight="1">
       <c r="A14" s="2">
         <v>44646.512648807868</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>44</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>32</v>
@@ -3402,7 +3411,7 @@
         <v>156</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>77</v>
@@ -3423,10 +3432,10 @@
         <v>0</v>
       </c>
       <c r="O14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>216</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>217</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>59</v>
@@ -3462,7 +3471,7 @@
         <v>12</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>16</v>
@@ -3489,7 +3498,7 @@
         <v>174</v>
       </c>
       <c r="AL14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AM14" s="1" t="s">
         <v>24</v>
@@ -3504,22 +3513,22 @@
         <v>26</v>
       </c>
       <c r="AQ14" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR14" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="AR14" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="AS14" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT14" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AU14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="AU14" s="1" t="s">
+      <c r="AV14" s="1" t="s">
         <v>223</v>
-      </c>
-      <c r="AV14" s="1" t="s">
-        <v>224</v>
       </c>
       <c r="AW14" s="1" t="s">
         <v>37</v>
@@ -3531,10 +3540,10 @@
         <v>30</v>
       </c>
       <c r="AZ14" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
-    <row r="15" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:52" ht="15.75" customHeight="1">
       <c r="A15" s="2">
         <v>44647.485230532402</v>
       </c>
@@ -3554,10 +3563,10 @@
         <v>32</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>227</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>77</v>
@@ -3578,7 +3587,7 @@
         <v>78</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>8</v>
@@ -3596,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W15" s="1" t="s">
         <v>15</v>
@@ -3653,7 +3662,7 @@
         <v>26</v>
       </c>
       <c r="AQ15" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AS15" s="1" t="s">
         <v>28</v>
@@ -3668,7 +3677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:52" ht="15.75" customHeight="1">
       <c r="A16" s="2">
         <v>44647.676722037038</v>
       </c>
@@ -3691,7 +3700,7 @@
         <v>156</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>5</v>
@@ -3712,7 +3721,7 @@
         <v>78</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>59</v>
@@ -3772,7 +3781,7 @@
         <v>174</v>
       </c>
       <c r="AL16" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AM16" s="1" t="s">
         <v>41</v>
@@ -3793,7 +3802,7 @@
         <v>28</v>
       </c>
       <c r="AT16" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AW16" s="1" t="s">
         <v>37</v>
@@ -3805,7 +3814,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:52" ht="15.75" customHeight="1">
       <c r="A17" s="2">
         <v>44647.921008333331</v>
       </c>
@@ -3828,7 +3837,7 @@
         <v>156</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>5</v>
@@ -3864,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W17" s="1" t="s">
         <v>15</v>
@@ -3918,13 +3927,13 @@
         <v>26</v>
       </c>
       <c r="AQ17" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AS17" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT17" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AW17" s="1" t="s">
         <v>15</v>
@@ -3936,7 +3945,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:52" ht="15.75" customHeight="1">
       <c r="A18" s="2">
         <v>44647.976546481485</v>
       </c>
@@ -3944,13 +3953,13 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>44</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>32</v>
@@ -3959,7 +3968,7 @@
         <v>156</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>77</v>
@@ -4049,7 +4058,7 @@
         <v>26</v>
       </c>
       <c r="AQ18" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="AS18" s="1" t="s">
         <v>28</v>
@@ -4064,7 +4073,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:52" ht="15.75" customHeight="1">
       <c r="A19" s="2">
         <v>44648.717444837966</v>
       </c>
@@ -4087,7 +4096,7 @@
         <v>156</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>394</v>
+        <v>382</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>33</v>
@@ -4141,7 +4150,7 @@
         <v>12</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AC19" s="1" t="s">
         <v>16</v>
@@ -4183,34 +4192,34 @@
         <v>27</v>
       </c>
       <c r="AR19" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="AS19" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT19" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="AU19" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="AU19" s="1" t="s">
+      <c r="AV19" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="AV19" s="1" t="s">
+      <c r="AW19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AX19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AY19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="AZ19" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="AW19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AX19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AY19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AZ19" s="1" t="s">
-        <v>243</v>
-      </c>
     </row>
-    <row r="20" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:52" ht="15.75" customHeight="1">
       <c r="A20" s="2">
         <v>44649.769038090279</v>
       </c>
@@ -4218,7 +4227,7 @@
         <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>44</v>
@@ -4233,7 +4242,7 @@
         <v>156</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>33</v>
@@ -4269,7 +4278,7 @@
         <v>0</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>12</v>
@@ -4287,7 +4296,7 @@
         <v>37</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="AC20" s="1" t="s">
         <v>48</v>
@@ -4308,13 +4317,13 @@
         <v>25</v>
       </c>
       <c r="AI20" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AK20" s="1" t="s">
         <v>174</v>
       </c>
       <c r="AL20" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AM20" s="1" t="s">
         <v>41</v>
@@ -4329,19 +4338,19 @@
         <v>26</v>
       </c>
       <c r="AQ20" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AS20" s="1" t="s">
         <v>82</v>
       </c>
       <c r="AT20" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="AU20" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="AU20" s="1" t="s">
+      <c r="AV20" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="AV20" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="AW20" s="1" t="s">
         <v>37</v>
@@ -4353,10 +4362,10 @@
         <v>37</v>
       </c>
       <c r="AZ20" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
-    <row r="21" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:52" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>44651.400174710652</v>
       </c>
@@ -4379,7 +4388,7 @@
         <v>156</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>77</v>
@@ -4400,7 +4409,7 @@
         <v>0</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P21" s="2">
         <v>43905</v>
@@ -4439,7 +4448,7 @@
         <v>37</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AC21" s="1" t="s">
         <v>48</v>
@@ -4469,7 +4478,7 @@
         <v>174</v>
       </c>
       <c r="AL21" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="AM21" s="1" t="s">
         <v>41</v>
@@ -4484,22 +4493,22 @@
         <v>41</v>
       </c>
       <c r="AQ21" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="AR21" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="AR21" s="1" t="s">
-        <v>256</v>
       </c>
       <c r="AS21" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="AU21" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="AU21" s="1" t="s">
+      <c r="AV21" s="1" t="s">
         <v>258</v>
-      </c>
-      <c r="AV21" s="1" t="s">
-        <v>259</v>
       </c>
       <c r="AW21" s="1" t="s">
         <v>37</v>
@@ -4511,10 +4520,10 @@
         <v>37</v>
       </c>
       <c r="AZ21" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
-    <row r="22" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:52" ht="15.75" customHeight="1">
       <c r="A22" s="2">
         <v>44669.433834733798</v>
       </c>
@@ -4537,7 +4546,7 @@
         <v>156</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>77</v>
@@ -4576,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W22" s="1" t="s">
         <v>12</v>
@@ -4633,19 +4642,19 @@
         <v>26</v>
       </c>
       <c r="AQ22" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AS22" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT22" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="AU22" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="AU22" s="1" t="s">
+      <c r="AV22" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="AV22" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="AW22" s="1" t="s">
         <v>12</v>
@@ -4657,7 +4666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:52" ht="15.75" customHeight="1">
       <c r="A23" s="2">
         <v>44669.463378217595</v>
       </c>
@@ -4680,7 +4689,7 @@
         <v>156</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>77</v>
@@ -4716,7 +4725,7 @@
         <v>0</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>195</v>
+        <v>11</v>
       </c>
       <c r="W23" s="1" t="s">
         <v>15</v>
@@ -4785,7 +4794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:52" ht="15.75" customHeight="1">
       <c r="A24" s="2">
         <v>44669.522761319444</v>
       </c>
@@ -4808,7 +4817,7 @@
         <v>156</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>77</v>
@@ -4883,7 +4892,7 @@
         <v>21</v>
       </c>
       <c r="AI24" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AK24" s="1" t="s">
         <v>174</v>
@@ -4901,7 +4910,7 @@
         <v>26</v>
       </c>
       <c r="AQ24" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="AS24" s="1" t="s">
         <v>28</v>
@@ -4916,7 +4925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:52" ht="15.75" customHeight="1">
       <c r="A25" s="2">
         <v>44669.675171030089</v>
       </c>
@@ -4939,7 +4948,7 @@
         <v>156</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>77</v>
@@ -4966,7 +4975,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T25" s="1" t="s">
         <v>10</v>
@@ -5047,7 +5056,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:52" ht="15.75" customHeight="1">
       <c r="A26" s="2">
         <v>44669.966824780087</v>
       </c>
@@ -5070,7 +5079,7 @@
         <v>156</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>77</v>
@@ -5100,7 +5109,7 @@
         <v>10</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="T26" s="1" t="s">
         <v>10</v>
@@ -5178,7 +5187,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:52" ht="15.75" customHeight="1">
       <c r="A27" s="2">
         <v>44669.968822025461</v>
       </c>
@@ -5201,7 +5210,7 @@
         <v>156</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>77</v>
@@ -5294,20 +5303,20 @@
         <v>26</v>
       </c>
       <c r="AQ27" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="AS27" s="1" t="s">
         <v>53</v>
       </c>
       <c r="AT27" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="AU27" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="AU27" s="1" t="s">
+      <c r="AV27" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="AV27" s="1" t="s">
-        <v>274</v>
-      </c>
       <c r="AW27" s="1" t="s">
         <v>15</v>
       </c>
@@ -5318,7 +5327,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:52" ht="15.75" customHeight="1">
       <c r="A28" s="2">
         <v>44670.671746284723</v>
       </c>
@@ -5341,7 +5350,7 @@
         <v>156</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>77</v>
@@ -5395,7 +5404,7 @@
         <v>37</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="AC28" s="1" t="s">
         <v>48</v>
@@ -5406,6 +5415,9 @@
       <c r="AE28" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="AF28" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="AG28" s="1" t="s">
         <v>25</v>
       </c>
@@ -5431,23 +5443,23 @@
         <v>26</v>
       </c>
       <c r="AQ28" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="AR28" s="1" t="s">
         <v>276</v>
-      </c>
-      <c r="AR28" s="1" t="s">
-        <v>277</v>
       </c>
       <c r="AS28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT28" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="AU28" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="AU28" s="1" t="s">
+      <c r="AV28" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="AV28" s="1" t="s">
-        <v>280</v>
-      </c>
       <c r="AW28" s="1" t="s">
         <v>12</v>
       </c>
@@ -5458,7 +5470,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:52" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>44670.771344768524</v>
       </c>
@@ -5481,7 +5493,7 @@
         <v>156</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>77</v>
@@ -5502,7 +5514,7 @@
         <v>45</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>59</v>
@@ -5538,7 +5550,7 @@
         <v>12</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="AC29" s="1" t="s">
         <v>48</v>
@@ -5559,7 +5571,7 @@
         <v>25</v>
       </c>
       <c r="AI29" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="AK29" s="1" t="s">
         <v>174</v>
@@ -5577,17 +5589,17 @@
         <v>26</v>
       </c>
       <c r="AQ29" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AS29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AT29" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="AV29" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="AV29" s="1" t="s">
-        <v>286</v>
-      </c>
       <c r="AW29" s="1" t="s">
         <v>15</v>
       </c>
@@ -5598,7 +5610,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:52" ht="15.75" customHeight="1">
       <c r="A30" s="2">
         <v>44754.453575532403</v>
       </c>
@@ -5621,7 +5633,7 @@
         <v>156</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>77</v>
@@ -5717,16 +5729,16 @@
         <v>41</v>
       </c>
       <c r="AQ30" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="AS30" s="1" t="s">
         <v>28</v>
       </c>
       <c r="AU30" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="AV30" s="1" t="s">
         <v>288</v>
-      </c>
-      <c r="AV30" s="1" t="s">
-        <v>289</v>
       </c>
       <c r="AW30" s="1" t="s">
         <v>37</v>
@@ -5738,7 +5750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:52" ht="15.75" customHeight="1">
       <c r="A31" s="2">
         <v>44879.894109953704</v>
       </c>
@@ -5761,7 +5773,7 @@
         <v>156</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>395</v>
+        <v>383</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>5</v>
@@ -5872,7 +5884,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:52" ht="15.75" customHeight="1">
       <c r="A32" s="2">
         <v>44880.347730717593</v>
       </c>
@@ -5895,7 +5907,7 @@
         <v>156</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>33</v>
@@ -6000,7 +6012,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:52" ht="15.75" customHeight="1">
       <c r="A33" s="2">
         <v>44881.627196759262</v>
       </c>
@@ -6023,7 +6035,7 @@
         <v>156</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>33</v>
@@ -6149,7 +6161,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:52" ht="15.75" customHeight="1">
       <c r="A34" s="2">
         <v>44883.582158321762</v>
       </c>
@@ -6172,7 +6184,7 @@
         <v>156</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>5</v>
@@ -6289,7 +6301,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="35" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:52" ht="15.75" customHeight="1">
       <c r="A35" s="2">
         <v>44885.785295578702</v>
       </c>
@@ -6312,7 +6324,7 @@
         <v>156</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>5</v>
@@ -6435,7 +6447,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="36" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:52" ht="15.75" customHeight="1">
       <c r="A36" s="2">
         <v>44885.839950104171</v>
       </c>
@@ -6581,7 +6593,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:52" ht="15.75" customHeight="1">
       <c r="A37" s="2">
         <v>44885.841205833334</v>
       </c>
@@ -6712,7 +6724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:52" ht="15.75" customHeight="1">
       <c r="A38" s="2">
         <v>44886.642705254635</v>
       </c>
@@ -6735,7 +6747,7 @@
         <v>156</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>5</v>
@@ -6867,7 +6879,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:52" ht="15.75" customHeight="1">
       <c r="A39" s="2">
         <v>44886.644437581017</v>
       </c>
@@ -6890,7 +6902,7 @@
         <v>101</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>33</v>
@@ -7010,7 +7022,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:52" ht="15.75" customHeight="1">
       <c r="A40" s="2">
         <v>44886.649916111113</v>
       </c>
@@ -7033,7 +7045,7 @@
         <v>156</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>33</v>
@@ -7138,7 +7150,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:52" ht="15.75" customHeight="1">
       <c r="A41" s="2">
         <v>44886.684875196763</v>
       </c>
@@ -7161,7 +7173,7 @@
         <v>101</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>33</v>
@@ -7287,7 +7299,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:52" ht="15.75" customHeight="1">
       <c r="A42" s="2">
         <v>44886.748539513894</v>
       </c>
@@ -7424,7 +7436,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:52" ht="15.75" customHeight="1">
       <c r="A43" s="2">
         <v>44886.767306041671</v>
       </c>
@@ -7564,7 +7576,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:52" ht="15.75" customHeight="1">
       <c r="A44" s="2">
         <v>44886.878623761571</v>
       </c>
@@ -7692,7 +7704,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:52" ht="15.75" customHeight="1">
       <c r="A45" s="2">
         <v>44886.924897337958</v>
       </c>
@@ -7820,7 +7832,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:52" ht="15.75" customHeight="1">
       <c r="A46" s="2">
         <v>44886.958313206022</v>
       </c>
@@ -7843,7 +7855,7 @@
         <v>156</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>33</v>
@@ -7957,7 +7969,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:52" ht="15.75" customHeight="1">
       <c r="A47" s="2">
         <v>44888.341911099538</v>
       </c>
@@ -7977,7 +7989,7 @@
         <v>32</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>138</v>
@@ -8112,7 +8124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:52" ht="15.75" customHeight="1">
       <c r="A48" s="2">
         <v>44895.541855706018</v>
       </c>
@@ -8135,7 +8147,7 @@
         <v>156</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>5</v>
@@ -8264,7 +8276,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:54" ht="15.75" customHeight="1">
       <c r="A49" s="2">
         <v>44899.894309016207</v>
       </c>
@@ -8287,7 +8299,7 @@
         <v>156</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>5</v>
@@ -8407,7 +8419,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:54" ht="15.75" customHeight="1">
       <c r="A50" s="2">
         <v>44900.956294351854</v>
       </c>
@@ -8430,7 +8442,7 @@
         <v>156</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>5</v>
@@ -8556,7 +8568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:54" ht="15.75" customHeight="1">
       <c r="A51" s="2">
         <v>44901.570091388887</v>
       </c>
@@ -8579,7 +8591,7 @@
         <v>156</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>5</v>
@@ -8696,7 +8708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:54" ht="15.75" customHeight="1">
       <c r="A52" s="7">
         <v>44907</v>
       </c>
@@ -8710,19 +8722,19 @@
         <v>44</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>32</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="J52" s="6">
         <v>44046</v>
@@ -8740,7 +8752,7 @@
         <v>10</v>
       </c>
       <c r="O52" s="8" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
       <c r="P52" s="4"/>
       <c r="Q52" s="4" t="s">
@@ -8777,7 +8789,7 @@
         <v>30</v>
       </c>
       <c r="AB52" s="4" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="AC52" s="4" t="s">
         <v>48</v>
@@ -8805,7 +8817,7 @@
         <v>23</v>
       </c>
       <c r="AL52" s="4" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="AM52" s="4" t="s">
         <v>62</v>
@@ -8820,22 +8832,22 @@
         <v>26</v>
       </c>
       <c r="AQ52" s="4" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="AR52" s="4" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="AS52" s="4" t="s">
         <v>82</v>
       </c>
       <c r="AT52" s="4" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="AU52" s="4" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
       <c r="AV52" s="4" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="AW52" s="4" t="s">
         <v>91</v>
@@ -8847,12 +8859,12 @@
         <v>91</v>
       </c>
       <c r="AZ52" s="4" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
       <c r="BA52" s="4"/>
       <c r="BB52" s="4"/>
     </row>
-    <row r="53" spans="1:54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:54" ht="15.75" customHeight="1">
       <c r="A53" s="7">
         <v>44908</v>
       </c>
@@ -8875,7 +8887,7 @@
         <v>156</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="I53" s="4" t="s">
         <v>33</v>
@@ -8933,7 +8945,7 @@
         <v>15</v>
       </c>
       <c r="AB53" s="4" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="AC53" s="4" t="s">
         <v>16</v>
@@ -8961,7 +8973,7 @@
         <v>23</v>
       </c>
       <c r="AL53" s="4" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="AM53" s="4" t="s">
         <v>24</v>
@@ -8976,22 +8988,22 @@
         <v>26</v>
       </c>
       <c r="AQ53" s="4" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="AR53" s="4" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="AS53" s="4" t="s">
         <v>53</v>
       </c>
       <c r="AT53" s="4" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="AU53" s="4" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
       <c r="AV53" s="4" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="AW53" s="4" t="s">
         <v>15</v>
@@ -9005,6 +9017,11 @@
       <c r="AZ53" s="4"/>
       <c r="BA53" s="4"/>
       <c r="BB53" s="4"/>
+    </row>
+    <row r="54" spans="1:54" ht="15.75" customHeight="1">
+      <c r="AZ54" t="s">
+        <v>393</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>